<commit_message>
Gantt and sprint update
</commit_message>
<xml_diff>
--- a/SprintBacklog/Sprint1.xlsx
+++ b/SprintBacklog/Sprint1.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="35">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -93,52 +93,52 @@
     <t>Create SQL Server database based on database diagram</t>
   </si>
   <si>
-    <t>Create PHP Querys for implementation in sprint</t>
-  </si>
-  <si>
-    <t>Create SQLite database for implementation in sprint</t>
-  </si>
-  <si>
     <t>3)  Ability for user to add, edit and delete recipes</t>
   </si>
   <si>
     <t>2) Ability to add a user</t>
   </si>
   <si>
-    <t>Add account</t>
-  </si>
-  <si>
     <t>Sign user in</t>
   </si>
   <si>
-    <t>Delete account</t>
-  </si>
-  <si>
-    <t>Edit recipe</t>
-  </si>
-  <si>
-    <t>Delete recipe</t>
-  </si>
-  <si>
-    <t>View recipe</t>
-  </si>
-  <si>
-    <t>Sign in/sign up pages</t>
-  </si>
-  <si>
     <t>Tues</t>
   </si>
   <si>
     <t xml:space="preserve">Sat </t>
   </si>
   <si>
-    <t>Add recipe</t>
-  </si>
-  <si>
     <t>Unit Tests</t>
   </si>
   <si>
     <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Create SQLite database for implementation in sprint (i.e. only tables needed for sprint)</t>
+  </si>
+  <si>
+    <t>Create PHP Querys for implementation in sprint  (i.e. only tables needed for sprint)</t>
+  </si>
+  <si>
+    <t>Basic add account</t>
+  </si>
+  <si>
+    <t>Delete account code</t>
+  </si>
+  <si>
+    <t>GUI page sign up/sign in and move add account code to GUI</t>
+  </si>
+  <si>
+    <t>Basic add recipe code</t>
+  </si>
+  <si>
+    <t>Add recipe code GUI</t>
+  </si>
+  <si>
+    <t>Exception and error catching</t>
+  </si>
+  <si>
+    <t>Sync code</t>
   </si>
 </sst>
 </file>
@@ -246,7 +246,7 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="122">
+  <dxfs count="66">
     <dxf>
       <fill>
         <patternFill>
@@ -313,13 +313,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -341,6 +334,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -390,13 +390,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -552,391 +545,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1112,8 +720,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="121"/>
-      <tableStyleElement type="headerRow" dxfId="120"/>
+      <tableStyleElement type="wholeTable" dxfId="65"/>
+      <tableStyleElement type="headerRow" dxfId="64"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1419,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W27"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1469,7 +1077,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>3</v>
@@ -1481,7 +1089,7 @@
         <v>5</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>7</v>
@@ -1516,7 +1124,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1566,37 +1174,37 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>8</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -1622,28 +1230,28 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <v>9</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1678,7 +1286,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>1</v>
@@ -1696,7 +1304,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>3</v>
@@ -1708,7 +1316,7 @@
         <v>5</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>7</v>
@@ -1734,28 +1342,28 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1790,91 +1398,174 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>17</v>
+      </c>
+      <c r="G13">
+        <v>17</v>
+      </c>
+      <c r="H13">
+        <v>17</v>
+      </c>
+      <c r="I13">
+        <v>17</v>
+      </c>
+      <c r="J13">
+        <v>17</v>
+      </c>
+      <c r="K13">
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
+      <c r="J15">
+        <v>7</v>
+      </c>
+      <c r="K15">
+        <v>7</v>
+      </c>
+      <c r="L15">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>1</v>
@@ -1892,7 +1583,7 @@
         <v>8</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>3</v>
@@ -1904,7 +1595,7 @@
         <v>5</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>7</v>
@@ -1930,7 +1621,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18">
         <v>10</v>
@@ -1942,25 +1633,25 @@
         <v>10</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1986,7 +1677,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B19">
         <v>10</v>
@@ -1998,25 +1689,25 @@
         <v>10</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -2037,444 +1728,358 @@
         <v>0</v>
       </c>
       <c r="R19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20">
-        <v>10</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20">
-        <v>10</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21">
-        <v>14</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="A21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D21">
-        <v>14</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="R24" s="3" t="s">
-        <v>6</v>
+      <c r="A24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B27">
-        <f>SUM(B5:B24)</f>
-        <v>101</v>
-      </c>
-      <c r="D27">
-        <f>SUM(D5:D24)</f>
+      <c r="B25">
+        <f>SUM(B5:B21)</f>
         <v>99</v>
       </c>
-      <c r="E27">
-        <f>SUM(E5:E24)</f>
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <f>SUM(F5:F24)</f>
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <f>SUM(G5:G24)</f>
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <f>SUM(H5:H24)</f>
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <f>SUM(I5:I24)</f>
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <f>SUM(J5:J24)</f>
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <f>SUM(K5:K24)</f>
-        <v>0</v>
+      <c r="D25">
+        <f t="shared" ref="D25:K25" si="0">SUM(D5:D21)</f>
+        <v>97</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:C7">
-    <cfRule type="containsText" dxfId="75" priority="94" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="59" priority="102" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="95" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="58" priority="103" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="96" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="57" priority="104" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C7">
-    <cfRule type="cellIs" dxfId="72" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="101" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="containsText" dxfId="55" priority="42" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="55" priority="50" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="43" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="54" priority="51" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="44" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="52" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="49" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="containsText" dxfId="51" priority="38" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="51" priority="46" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="39" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="50" priority="47" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="40" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="49" priority="48" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="48" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="45" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="containsText" dxfId="47" priority="42" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="43" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="44" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="cellIs" dxfId="44" priority="41" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="cellIs" dxfId="43" priority="13" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="containsText" dxfId="47" priority="34" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="42" priority="38" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="35" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="41" priority="39" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="36" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="40" priority="40" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="44" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="40" priority="9" operator="equal">
+  <conditionalFormatting sqref="C15">
+    <cfRule type="containsText" dxfId="38" priority="34" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="containsText" dxfId="34" priority="26" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="28" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="cellIs" dxfId="31" priority="25" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C22)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="39" priority="30" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="31" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="32" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="36" priority="29" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="containsText" dxfId="35" priority="26" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",C14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="27" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",C14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="28" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",C14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="32" priority="25" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="31" priority="22" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",C18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="23" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",C18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="24" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",C18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="28" priority="21" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="27" priority="18" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",C19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="19" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",C19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",C19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="24" priority="17" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="23" priority="14" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",C20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",C20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",C20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="containsText" dxfId="19" priority="10" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",C21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="11" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",C21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="12" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",C21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",C25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",C25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",C25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",C26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",C26)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",C26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
@@ -2483,7 +2088,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3">
       <formula1>To_Do</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7 C11:C14 C18:C21 C25:C26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7 C18:C19 C22:C24 C11:C15">
       <formula1>Todos</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>